<commit_message>
implemented classifier. Hybrid class available.
</commit_message>
<xml_diff>
--- a/src/data/qb_zulehner_toronto.xlsx
+++ b/src/data/qb_zulehner_toronto.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SuhasVittal/Documents/programming/qcr/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{884C5DEF-D7EC-534D-BB74-9C7693917E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C491A8-86D2-C34F-8638-1A3687C940A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="560" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="780" yWindow="560" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="qb_zulehner_toronto" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>SABRE CNOTs</t>
   </si>
@@ -235,12 +257,18 @@
   </si>
   <si>
     <t>improvement</t>
+  </si>
+  <si>
+    <t>Hybrid CNOTs</t>
+  </si>
+  <si>
+    <t>Hybrid Depth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1074,16 +1102,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="P59" sqref="P59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1120,8 +1148,14 @@
       <c r="M1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1161,8 +1195,16 @@
       <c r="M2">
         <v>5.8511970000001403E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2">
+        <f>MIN(B2,E2,H2)</f>
+        <v>165</v>
+      </c>
+      <c r="O2" cm="1">
+        <f t="array" ref="O2">INDEX(CHOOSE({1,2,3},C2,F2,I2), MATCH(N2, CHOOSE({1,2,3},B2,E2,H2), 0))</f>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1202,8 +1244,16 @@
       <c r="M3">
         <v>3.9629309999995102E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3">
+        <f t="shared" ref="N3:N55" si="0">MIN(B3,E3,H3)</f>
+        <v>831</v>
+      </c>
+      <c r="O3" cm="1">
+        <f t="array" ref="O3">INDEX(CHOOSE({1,2,3},C3,F3,I3), MATCH(N3, CHOOSE({1,2,3},B3,E3,H3), 0))</f>
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1243,8 +1293,16 @@
       <c r="M4">
         <v>1.00690579999991E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>321</v>
+      </c>
+      <c r="O4" cm="1">
+        <f t="array" ref="O4">INDEX(CHOOSE({1,2,3},C4,F4,I4), MATCH(N4, CHOOSE({1,2,3},B4,E4,H4), 0))</f>
+        <v>595</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1284,8 +1342,16 @@
       <c r="M5">
         <v>0.20110658800012901</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>3159</v>
+      </c>
+      <c r="O5" cm="1">
+        <f t="array" ref="O5">INDEX(CHOOSE({1,2,3},C5,F5,I5), MATCH(N5, CHOOSE({1,2,3},B5,E5,H5), 0))</f>
+        <v>4811</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1325,8 +1391,16 @@
       <c r="M6">
         <v>3.9720019999549497E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>129</v>
+      </c>
+      <c r="O6" cm="1">
+        <f t="array" ref="O6">INDEX(CHOOSE({1,2,3},C6,F6,I6), MATCH(N6, CHOOSE({1,2,3},B6,E6,H6), 0))</f>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1366,8 +1440,16 @@
       <c r="M7">
         <v>1.9497827999657599E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>375</v>
+      </c>
+      <c r="O7" cm="1">
+        <f t="array" ref="O7">INDEX(CHOOSE({1,2,3},C7,F7,I7), MATCH(N7, CHOOSE({1,2,3},B7,E7,H7), 0))</f>
+        <v>633</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1407,8 +1489,16 @@
       <c r="M8">
         <v>2.1029365000231299E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>183</v>
+      </c>
+      <c r="O8" cm="1">
+        <f t="array" ref="O8">INDEX(CHOOSE({1,2,3},C8,F8,I8), MATCH(N8, CHOOSE({1,2,3},B8,E8,H8), 0))</f>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1448,8 +1538,16 @@
       <c r="M9">
         <v>8.0501039999944596E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>843</v>
+      </c>
+      <c r="O9" cm="1">
+        <f t="array" ref="O9">INDEX(CHOOSE({1,2,3},C9,F9,I9), MATCH(N9, CHOOSE({1,2,3},B9,E9,H9), 0))</f>
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1489,8 +1587,16 @@
       <c r="M10">
         <v>1.42760200001248E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>261</v>
+      </c>
+      <c r="O10" cm="1">
+        <f t="array" ref="O10">INDEX(CHOOSE({1,2,3},C10,F10,I10), MATCH(N10, CHOOSE({1,2,3},B10,E10,H10), 0))</f>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1530,8 +1636,16 @@
       <c r="M11">
         <v>1.19636499998705E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>291</v>
+      </c>
+      <c r="O11" cm="1">
+        <f t="array" ref="O11">INDEX(CHOOSE({1,2,3},C11,F11,I11), MATCH(N11, CHOOSE({1,2,3},B11,E11,H11), 0))</f>
+        <v>519</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1571,8 +1685,16 @@
       <c r="M12">
         <v>0.36324510100075702</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>3270</v>
+      </c>
+      <c r="O12" cm="1">
+        <f t="array" ref="O12">INDEX(CHOOSE({1,2,3},C12,F12,I12), MATCH(N12, CHOOSE({1,2,3},B12,E12,H12), 0))</f>
+        <v>5030</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1612,8 +1734,16 @@
       <c r="M13">
         <v>1.5799838000020799E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+      <c r="O13" cm="1">
+        <f t="array" ref="O13">INDEX(CHOOSE({1,2,3},C13,F13,I13), MATCH(N13, CHOOSE({1,2,3},B13,E13,H13), 0))</f>
+        <v>409</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1653,8 +1783,16 @@
       <c r="M14">
         <v>6.2672441000358903E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>444</v>
+      </c>
+      <c r="O14" cm="1">
+        <f t="array" ref="O14">INDEX(CHOOSE({1,2,3},C14,F14,I14), MATCH(N14, CHOOSE({1,2,3},B14,E14,H14), 0))</f>
+        <v>635</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1694,8 +1832,16 @@
       <c r="M15">
         <v>2.8591600999789E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>354</v>
+      </c>
+      <c r="O15" cm="1">
+        <f t="array" ref="O15">INDEX(CHOOSE({1,2,3},C15,F15,I15), MATCH(N15, CHOOSE({1,2,3},B15,E15,H15), 0))</f>
+        <v>566</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1735,8 +1881,16 @@
       <c r="M16">
         <v>0.23902277400065899</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>3072</v>
+      </c>
+      <c r="O16" cm="1">
+        <f t="array" ref="O16">INDEX(CHOOSE({1,2,3},C16,F16,I16), MATCH(N16, CHOOSE({1,2,3},B16,E16,H16), 0))</f>
+        <v>4539</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1776,8 +1930,16 @@
       <c r="M17">
         <v>2.74280840003484E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>516</v>
+      </c>
+      <c r="O17" cm="1">
+        <f t="array" ref="O17">INDEX(CHOOSE({1,2,3},C17,F17,I17), MATCH(N17, CHOOSE({1,2,3},B17,E17,H17), 0))</f>
+        <v>831</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1817,8 +1979,16 @@
       <c r="M18">
         <v>1.87160720006431E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>243</v>
+      </c>
+      <c r="O18" cm="1">
+        <f t="array" ref="O18">INDEX(CHOOSE({1,2,3},C18,F18,I18), MATCH(N18, CHOOSE({1,2,3},B18,E18,H18), 0))</f>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1858,8 +2028,16 @@
       <c r="M19">
         <v>9.3878219000543994E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>1674</v>
+      </c>
+      <c r="O19" cm="1">
+        <f t="array" ref="O19">INDEX(CHOOSE({1,2,3},C19,F19,I19), MATCH(N19, CHOOSE({1,2,3},B19,E19,H19), 0))</f>
+        <v>2646</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1899,8 +2077,16 @@
       <c r="M20">
         <v>1.2441898999895701E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>237</v>
+      </c>
+      <c r="O20" cm="1">
+        <f t="array" ref="O20">INDEX(CHOOSE({1,2,3},C20,F20,I20), MATCH(N20, CHOOSE({1,2,3},B20,E20,H20), 0))</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1940,8 +2126,16 @@
       <c r="M21">
         <v>1.8804338999871099E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>432</v>
+      </c>
+      <c r="O21" cm="1">
+        <f t="array" ref="O21">INDEX(CHOOSE({1,2,3},C21,F21,I21), MATCH(N21, CHOOSE({1,2,3},B21,E21,H21), 0))</f>
+        <v>771</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1981,8 +2175,16 @@
       <c r="M22">
         <v>1.5253812000082601E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>348</v>
+      </c>
+      <c r="O22" cm="1">
+        <f t="array" ref="O22">INDEX(CHOOSE({1,2,3},C22,F22,I22), MATCH(N22, CHOOSE({1,2,3},B22,E22,H22), 0))</f>
+        <v>639</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2022,8 +2224,16 @@
       <c r="M23">
         <v>2.28804509997644E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>567</v>
+      </c>
+      <c r="O23" cm="1">
+        <f t="array" ref="O23">INDEX(CHOOSE({1,2,3},C23,F23,I23), MATCH(N23, CHOOSE({1,2,3},B23,E23,H23), 0))</f>
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2063,8 +2273,16 @@
       <c r="M24">
         <v>6.96768649995647E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>1488</v>
+      </c>
+      <c r="O24" cm="1">
+        <f t="array" ref="O24">INDEX(CHOOSE({1,2,3},C24,F24,I24), MATCH(N24, CHOOSE({1,2,3},B24,E24,H24), 0))</f>
+        <v>2521</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -2104,8 +2322,16 @@
       <c r="M25">
         <v>1.16643969995493E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>177</v>
+      </c>
+      <c r="O25" cm="1">
+        <f t="array" ref="O25">INDEX(CHOOSE({1,2,3},C25,F25,I25), MATCH(N25, CHOOSE({1,2,3},B25,E25,H25), 0))</f>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -2145,8 +2371,16 @@
       <c r="M26">
         <v>7.0906152999668806E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>1413</v>
+      </c>
+      <c r="O26" cm="1">
+        <f t="array" ref="O26">INDEX(CHOOSE({1,2,3},C26,F26,I26), MATCH(N26, CHOOSE({1,2,3},B26,E26,H26), 0))</f>
+        <v>2441</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -2186,8 +2420,16 @@
       <c r="M27">
         <v>1.0660703999746999E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>174</v>
+      </c>
+      <c r="O27" cm="1">
+        <f t="array" ref="O27">INDEX(CHOOSE({1,2,3},C27,F27,I27), MATCH(N27, CHOOSE({1,2,3},B27,E27,H27), 0))</f>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -2227,8 +2469,16 @@
       <c r="M28">
         <v>1.3307342999723901E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="O28" cm="1">
+        <f t="array" ref="O28">INDEX(CHOOSE({1,2,3},C28,F28,I28), MATCH(N28, CHOOSE({1,2,3},B28,E28,H28), 0))</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -2268,8 +2518,16 @@
       <c r="M29">
         <v>1.5520383999501E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N29">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="O29" cm="1">
+        <f t="array" ref="O29">INDEX(CHOOSE({1,2,3},C29,F29,I29), MATCH(N29, CHOOSE({1,2,3},B29,E29,H29), 0))</f>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -2309,8 +2567,16 @@
       <c r="M30">
         <v>5.5452040005547999E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="O30" cm="1">
+        <f t="array" ref="O30">INDEX(CHOOSE({1,2,3},C30,F30,I30), MATCH(N30, CHOOSE({1,2,3},B30,E30,H30), 0))</f>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2350,8 +2616,16 @@
       <c r="M31">
         <v>1.20457470002293E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N31">
+        <f t="shared" si="0"/>
+        <v>273</v>
+      </c>
+      <c r="O31" cm="1">
+        <f t="array" ref="O31">INDEX(CHOOSE({1,2,3},C31,F31,I31), MATCH(N31, CHOOSE({1,2,3},B31,E31,H31), 0))</f>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -2391,8 +2665,16 @@
       <c r="M32">
         <v>4.8762460000943897E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="O32" cm="1">
+        <f t="array" ref="O32">INDEX(CHOOSE({1,2,3},C32,F32,I32), MATCH(N32, CHOOSE({1,2,3},B32,E32,H32), 0))</f>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -2432,8 +2714,16 @@
       <c r="M33">
         <v>1.2706864999927301E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N33">
+        <f t="shared" si="0"/>
+        <v>219</v>
+      </c>
+      <c r="O33" cm="1">
+        <f t="array" ref="O33">INDEX(CHOOSE({1,2,3},C33,F33,I33), MATCH(N33, CHOOSE({1,2,3},B33,E33,H33), 0))</f>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -2473,8 +2763,16 @@
       <c r="M34">
         <v>8.5336809997897892E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N34">
+        <f t="shared" si="0"/>
+        <v>177</v>
+      </c>
+      <c r="O34" cm="1">
+        <f t="array" ref="O34">INDEX(CHOOSE({1,2,3},C34,F34,I34), MATCH(N34, CHOOSE({1,2,3},B34,E34,H34), 0))</f>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -2514,8 +2812,16 @@
       <c r="M35">
         <v>7.1532399997522502E-3</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N35">
+        <f t="shared" si="0"/>
+        <v>189</v>
+      </c>
+      <c r="O35" cm="1">
+        <f t="array" ref="O35">INDEX(CHOOSE({1,2,3},C35,F35,I35), MATCH(N35, CHOOSE({1,2,3},B35,E35,H35), 0))</f>
+        <v>349</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -2555,8 +2861,16 @@
       <c r="M36">
         <v>1.9217930999730001E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N36">
+        <f t="shared" si="0"/>
+        <v>579</v>
+      </c>
+      <c r="O36" cm="1">
+        <f t="array" ref="O36">INDEX(CHOOSE({1,2,3},C36,F36,I36), MATCH(N36, CHOOSE({1,2,3},B36,E36,H36), 0))</f>
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -2596,8 +2910,16 @@
       <c r="M37">
         <v>1.30382510005802E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N37">
+        <f t="shared" si="0"/>
+        <v>441</v>
+      </c>
+      <c r="O37" cm="1">
+        <f t="array" ref="O37">INDEX(CHOOSE({1,2,3},C37,F37,I37), MATCH(N37, CHOOSE({1,2,3},B37,E37,H37), 0))</f>
+        <v>731</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -2637,8 +2959,16 @@
       <c r="M38">
         <v>4.0882848000364902E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N38">
+        <f t="shared" si="0"/>
+        <v>1065</v>
+      </c>
+      <c r="O38" cm="1">
+        <f t="array" ref="O38">INDEX(CHOOSE({1,2,3},C38,F38,I38), MATCH(N38, CHOOSE({1,2,3},B38,E38,H38), 0))</f>
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -2678,8 +3008,16 @@
       <c r="M39">
         <v>9.9508869998317095E-3</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N39">
+        <f t="shared" si="0"/>
+        <v>261</v>
+      </c>
+      <c r="O39" cm="1">
+        <f t="array" ref="O39">INDEX(CHOOSE({1,2,3},C39,F39,I39), MATCH(N39, CHOOSE({1,2,3},B39,E39,H39), 0))</f>
+        <v>457</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -2719,8 +3057,16 @@
       <c r="M40">
         <v>1.27495450005881E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N40">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="O40" cm="1">
+        <f t="array" ref="O40">INDEX(CHOOSE({1,2,3},C40,F40,I40), MATCH(N40, CHOOSE({1,2,3},B40,E40,H40), 0))</f>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -2760,8 +3106,16 @@
       <c r="M41">
         <v>4.36377589994663E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N41">
+        <f t="shared" si="0"/>
+        <v>1002</v>
+      </c>
+      <c r="O41" cm="1">
+        <f t="array" ref="O41">INDEX(CHOOSE({1,2,3},C41,F41,I41), MATCH(N41, CHOOSE({1,2,3},B41,E41,H41), 0))</f>
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -2801,8 +3155,16 @@
       <c r="M42">
         <v>3.9030692998494397E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N42">
+        <f t="shared" si="0"/>
+        <v>1077</v>
+      </c>
+      <c r="O42" cm="1">
+        <f t="array" ref="O42">INDEX(CHOOSE({1,2,3},C42,F42,I42), MATCH(N42, CHOOSE({1,2,3},B42,E42,H42), 0))</f>
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -2842,8 +3204,16 @@
       <c r="M43">
         <v>9.12485249991732E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N43">
+        <f t="shared" si="0"/>
+        <v>1890</v>
+      </c>
+      <c r="O43" cm="1">
+        <f t="array" ref="O43">INDEX(CHOOSE({1,2,3},C43,F43,I43), MATCH(N43, CHOOSE({1,2,3},B43,E43,H43), 0))</f>
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -2883,8 +3253,16 @@
       <c r="M44">
         <v>2.9529948000344999E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N44">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="O44" cm="1">
+        <f t="array" ref="O44">INDEX(CHOOSE({1,2,3},C44,F44,I44), MATCH(N44, CHOOSE({1,2,3},B44,E44,H44), 0))</f>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -2924,8 +3302,16 @@
       <c r="M45">
         <v>2.00461559998075E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N45">
+        <f t="shared" si="0"/>
+        <v>297</v>
+      </c>
+      <c r="O45" cm="1">
+        <f t="array" ref="O45">INDEX(CHOOSE({1,2,3},C45,F45,I45), MATCH(N45, CHOOSE({1,2,3},B45,E45,H45), 0))</f>
+        <v>568</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -2965,8 +3351,16 @@
       <c r="M46">
         <v>1.17254760007199E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N46">
+        <f t="shared" si="0"/>
+        <v>207</v>
+      </c>
+      <c r="O46" cm="1">
+        <f t="array" ref="O46">INDEX(CHOOSE({1,2,3},C46,F46,I46), MATCH(N46, CHOOSE({1,2,3},B46,E46,H46), 0))</f>
+        <v>359</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -3006,8 +3400,16 @@
       <c r="M47">
         <v>2.0540616000289402E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N47">
+        <f t="shared" si="0"/>
+        <v>264</v>
+      </c>
+      <c r="O47" cm="1">
+        <f t="array" ref="O47">INDEX(CHOOSE({1,2,3},C47,F47,I47), MATCH(N47, CHOOSE({1,2,3},B47,E47,H47), 0))</f>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -3047,8 +3449,16 @@
       <c r="M48">
         <v>2.7093456999864401E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N48">
+        <f t="shared" si="0"/>
+        <v>987</v>
+      </c>
+      <c r="O48" cm="1">
+        <f t="array" ref="O48">INDEX(CHOOSE({1,2,3},C48,F48,I48), MATCH(N48, CHOOSE({1,2,3},B48,E48,H48), 0))</f>
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -3088,8 +3498,16 @@
       <c r="M49">
         <v>1.21847059999709E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N49">
+        <f t="shared" si="0"/>
+        <v>303</v>
+      </c>
+      <c r="O49" cm="1">
+        <f t="array" ref="O49">INDEX(CHOOSE({1,2,3},C49,F49,I49), MATCH(N49, CHOOSE({1,2,3},B49,E49,H49), 0))</f>
+        <v>464</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -3129,8 +3547,16 @@
       <c r="M50">
         <v>1.57289979997585E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N50">
+        <f t="shared" si="0"/>
+        <v>405</v>
+      </c>
+      <c r="O50" cm="1">
+        <f t="array" ref="O50">INDEX(CHOOSE({1,2,3},C50,F50,I50), MATCH(N50, CHOOSE({1,2,3},B50,E50,H50), 0))</f>
+        <v>577</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>61</v>
       </c>
@@ -3170,8 +3596,16 @@
       <c r="M51">
         <v>0.171042658001169</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N51">
+        <f t="shared" si="0"/>
+        <v>2805</v>
+      </c>
+      <c r="O51" cm="1">
+        <f t="array" ref="O51">INDEX(CHOOSE({1,2,3},C51,F51,I51), MATCH(N51, CHOOSE({1,2,3},B51,E51,H51), 0))</f>
+        <v>4417</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>62</v>
       </c>
@@ -3211,8 +3645,16 @@
       <c r="M52">
         <v>1.9059222999203401E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N52">
+        <f t="shared" si="0"/>
+        <v>540</v>
+      </c>
+      <c r="O52" cm="1">
+        <f t="array" ref="O52">INDEX(CHOOSE({1,2,3},C52,F52,I52), MATCH(N52, CHOOSE({1,2,3},B52,E52,H52), 0))</f>
+        <v>914</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>63</v>
       </c>
@@ -3252,8 +3694,16 @@
       <c r="M53">
         <v>3.2194392000747002E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N53">
+        <f t="shared" si="0"/>
+        <v>798</v>
+      </c>
+      <c r="O53" cm="1">
+        <f t="array" ref="O53">INDEX(CHOOSE({1,2,3},C53,F53,I53), MATCH(N53, CHOOSE({1,2,3},B53,E53,H53), 0))</f>
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -3293,8 +3743,16 @@
       <c r="M54">
         <v>2.27705050001532E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N54">
+        <f t="shared" si="0"/>
+        <v>462</v>
+      </c>
+      <c r="O54" cm="1">
+        <f t="array" ref="O54">INDEX(CHOOSE({1,2,3},C54,F54,I54), MATCH(N54, CHOOSE({1,2,3},B54,E54,H54), 0))</f>
+        <v>819</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -3334,8 +3792,16 @@
       <c r="M55">
         <v>1.3993664999361499E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N55">
+        <f t="shared" si="0"/>
+        <v>204</v>
+      </c>
+      <c r="O55" cm="1">
+        <f t="array" ref="O55">INDEX(CHOOSE({1,2,3},C55,F55,I55), MATCH(N55, CHOOSE({1,2,3},B55,E55,H55), 0))</f>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -3344,51 +3810,59 @@
         <v>701.22222222222217</v>
       </c>
       <c r="C56">
-        <f t="shared" ref="C56:M56" si="0">AVERAGE(C2:C55)</f>
+        <f t="shared" ref="C56:O56" si="1">AVERAGE(C2:C55)</f>
         <v>1138.2037037037037</v>
       </c>
       <c r="D56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.3602583783703614</v>
       </c>
       <c r="E56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>718.11111111111109</v>
       </c>
       <c r="F56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>907.07407407407402</v>
       </c>
       <c r="G56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.9988574223332609</v>
       </c>
       <c r="H56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>689.22222222222217</v>
       </c>
       <c r="I56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1127.2037037037037</v>
       </c>
       <c r="J56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>153.39119203112958</v>
       </c>
       <c r="K56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>753.83333333333337</v>
       </c>
       <c r="L56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1093.962962962963</v>
       </c>
       <c r="M56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.138692142593265E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N56">
+        <f t="shared" si="1"/>
+        <v>679.83333333333337</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="1"/>
+        <v>1080.851851851852</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -3439,6 +3913,14 @@
       <c r="M57">
         <f>($D$56 - M56)/$D$56</f>
         <v>0.88511878165568969</v>
+      </c>
+      <c r="N57">
+        <f>($B$56 - N56)/$B$56</f>
+        <v>3.0502297575661419E-2</v>
+      </c>
+      <c r="O57">
+        <f>($C$56 - O56)/$C$56</f>
+        <v>5.0388038332004517E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>